<commit_message>
started burnt chopped wood and minor edits to aspen meadow
</commit_message>
<xml_diff>
--- a/data/clean/burnt_chopped_wood.xlsx
+++ b/data/clean/burnt_chopped_wood.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie Frazer\Documents\ESS500_ForestCarbon\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0767935-BFBF-4331-8D45-ABC2A7980B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFB558D-324B-4830-8DCF-F84C12203DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="2808" windowWidth="12960" windowHeight="7824" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F24 % Cover" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>Litter</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Relatvie Frequency (# encounter in relation to other types of cover)</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t># of time occurred / # of events that can occur</t>
+  </si>
+  <si>
+    <t>GroundCover</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -219,7 +219,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -680,28 +680,28 @@
         <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -778,28 +778,28 @@
         <v>80</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -870,7 +870,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -893,40 +893,40 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1341,28 +1341,28 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1386,6 +1386,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -1650,9 +1653,6 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
       <c r="H10">
         <v>10</v>
       </c>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1677,18 +1677,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F26462-0CEA-4841-9244-0BEF5EBE4692}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -1749,8 +1752,7 @@
         <v>19</v>
       </c>
       <c r="K3" s="2">
-        <f>(3/29)*100</f>
-        <v>10.344827586206897</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1782,8 +1784,7 @@
         <v>19</v>
       </c>
       <c r="K4" s="2">
-        <f>(8/29)*100</f>
-        <v>27.586206896551722</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1815,8 +1816,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <f>(1/29)*100</f>
-        <v>3.4482758620689653</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1848,8 +1848,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2">
-        <f>(1/29)*100</f>
-        <v>3.4482758620689653</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1881,8 +1880,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2">
-        <f>(6/29)*100</f>
-        <v>20.689655172413794</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1914,8 +1912,7 @@
         <v>27</v>
       </c>
       <c r="K8" s="2">
-        <f>(8/29)*100</f>
-        <v>27.586206896551722</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1947,17 +1944,13 @@
         <v>22</v>
       </c>
       <c r="K9" s="2">
-        <f>(2/29)*100</f>
-        <v>6.8965517241379306</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
       <c r="H10">
         <v>23</v>
       </c>
@@ -1970,7 +1963,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1982,18 +1975,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7CB3220-D5BE-4019-80C2-449396573435}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
       <c r="B2">
         <v>1996</v>
       </c>
@@ -2253,9 +2249,6 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
       <c r="H10">
         <v>17.5</v>
       </c>
@@ -2268,7 +2261,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>